<commit_message>
Add hex explain to the bytes.
</commit_message>
<xml_diff>
--- a/Frame Explained.xlsx
+++ b/Frame Explained.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chihong\Documents\Repos\Makerfabs-ESP32-UWB-DW3000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NI\Documents\CC\UWB\UWB-DW3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7178949-E68E-4687-8B60-BCE6227467F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2083AE0-AEF7-465D-B6BD-2B27C4DA50DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="15600" activeTab="1" xr2:uid="{E1680DE1-9DBE-4A93-A31B-6A32B9863B9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E1680DE1-9DBE-4A93-A31B-6A32B9863B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -153,18 +153,6 @@
     <t>0xDE</t>
   </si>
   <si>
-    <t>'W'</t>
-  </si>
-  <si>
-    <t>'A'</t>
-  </si>
-  <si>
-    <t>'V'</t>
-  </si>
-  <si>
-    <t>'E'</t>
-  </si>
-  <si>
     <t>0xE0</t>
   </si>
   <si>
@@ -307,6 +295,18 @@
   </si>
   <si>
     <t>(Treply anchor)</t>
+  </si>
+  <si>
+    <t>W' (0x57)</t>
+  </si>
+  <si>
+    <t>A' (0x41)</t>
+  </si>
+  <si>
+    <t>V' (0x56)</t>
+  </si>
+  <si>
+    <t>E' (0x45)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1540249</xdr:colOff>
+      <xdr:colOff>1226484</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>172091</xdr:rowOff>
     </xdr:to>
@@ -452,7 +452,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>316371</xdr:colOff>
+      <xdr:colOff>2606</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>92489</xdr:rowOff>
     </xdr:to>
@@ -790,7 +790,7 @@
   <dimension ref="A2:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
         <v>450</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -1078,46 +1078,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BE20B6-9AA9-46AC-A707-8D5AC88528B3}">
   <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="6" width="2.5703125" customWidth="1"/>
-    <col min="7" max="8" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.85546875" customWidth="1"/>
     <col min="10" max="21" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1128,7 +1129,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1145,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1162,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -1171,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1182,7 +1183,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -1191,7 +1192,7 @@
         <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1202,7 +1203,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -1211,87 +1212,87 @@
         <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
+      <c r="B9" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>40</v>
+      <c r="H9" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>39</v>
+      <c r="B10" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>41</v>
+      <c r="H10" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
+      <c r="B11" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G11">
         <v>7</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>38</v>
+      <c r="H11" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>41</v>
+      <c r="B12" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>39</v>
+      <c r="H12" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1299,10 +1300,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G13">
         <v>9</v>
@@ -1311,7 +1312,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1322,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1331,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1342,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G15">
         <v>11</v>
@@ -1351,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1362,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1373,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1384,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1395,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1406,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1417,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,32 +1440,32 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>25</v>
@@ -1472,131 +1473,131 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J32" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J34" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J35" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J36" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J37" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J38" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J39" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J40" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J41" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J42" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J43" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J44" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J45" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J46" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J47" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J48" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="N52" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="N53" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="N54" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="N55" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="N56" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="N57" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -1620,13 +1621,13 @@
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="N64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="N65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>